<commit_message>
Add new code function
</commit_message>
<xml_diff>
--- a/src/main/java/util/excelfile/Input.xlsx
+++ b/src/main/java/util/excelfile/Input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caohieu/Desktop/HotelManagementSystem/src/main/java/util/excelfile/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caohieu/Downloads/Hotel-Booking-master/hotel/src/main/java/util/excelfile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDA4625-5F75-B446-876F-46253E21E230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DC8BE0-03AC-1E4B-A01E-1C1CB6AA3326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="1760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6980" yWindow="1840" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Client insert" sheetId="6" r:id="rId1"/>
@@ -752,6 +752,619 @@
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6"/>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="22"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6"/>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6"/>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF333333"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6"/>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
         <u/>
         <vertAlign val="baseline"/>
         <sz val="20"/>
@@ -780,17 +1393,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -817,608 +1419,6 @@
           <color theme="6" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="6"/>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="22"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="6"/>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="6"/>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color rgb="FF333333"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="6"/>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1566,66 +1566,66 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ID CARD" dataDxfId="42"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="FULL NAME" dataDxfId="41"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ADDRESS" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="TEL" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="EMAIL" dataDxfId="0" dataCellStyle="Hyperlink"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="NOTE" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="TEL" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="EMAIL" dataDxfId="38" dataCellStyle="Hyperlink"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="NOTE" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table6" displayName="Table6" ref="A1:F3" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table6" displayName="Table6" ref="A1:F3" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33">
   <autoFilter ref="A1:F3" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="HOTEL ID" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="NAME" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="STAR LEVEL" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ADDRESS" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="CITY" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="DESCRIPTION" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="HOTEL ID" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="NAME" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="STAR LEVEL" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ADDRESS" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="CITY" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="DESCRIPTION" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table7" displayName="Table7" ref="A1:F31" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table7" displayName="Table7" ref="A1:F31" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23">
   <autoFilter ref="A1:F31" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name=" ROOM ID" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="HOTEL ID" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="NAME" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="TYPE" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="PRICE" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="DESCRIPTION" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name=" ROOM ID" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="HOTEL ID" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="NAME" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="TYPE" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="PRICE" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="DESCRIPTION" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table8" displayName="Table8" ref="A1:D11" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table8" displayName="Table8" ref="A1:D11" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13">
   <autoFilter ref="A1:D11" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="ID" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="NAME" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="UNITY" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="PRICE" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="ID" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="NAME" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="UNITY" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="PRICE" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table9" displayName="Table9" ref="A1:E11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table9" displayName="Table9" ref="A1:E11" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
   <autoFilter ref="A1:E11" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="ID" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="USER NAME" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="FULL NAME" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="PASSWORD" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="POSITION" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="ID" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="USER NAME" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="FULL NAME" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="PASSWORD" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="POSITION" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1931,7 +1931,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2359,8 +2359,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2946,7 +2946,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>

</xml_diff>